<commit_message>
added relative ratio to xls
</commit_message>
<xml_diff>
--- a/histologicalslides/BleuAlcyan/test/resultAUC.xlsx
+++ b/histologicalslides/BleuAlcyan/test/resultAUC.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="resultAUC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>AUCred</t>
   </si>
@@ -115,6 +115,24 @@
   </si>
   <si>
     <t>FLNA 492-21 3W BA - 2019-02-06 10,24,42,tifAbsoluteBA,csv</t>
+  </si>
+  <si>
+    <t>relwidthtiers1</t>
+  </si>
+  <si>
+    <t>relwidthtiers2</t>
+  </si>
+  <si>
+    <t>relwidthtiers3</t>
+  </si>
+  <si>
+    <t>relratiotiers1</t>
+  </si>
+  <si>
+    <t>relratiotier2</t>
+  </si>
+  <si>
+    <t>relratiotiers3</t>
   </si>
 </sst>
 </file>
@@ -921,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +950,7 @@
     <col min="1" max="4" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -987,8 +1005,26 @@
       <c r="R1" t="s">
         <v>13</v>
       </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V1" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1043,8 +1079,32 @@
       <c r="R2">
         <v>29.5519679920464</v>
       </c>
+      <c r="S2">
+        <f>J2/SUM(J2:L2)</f>
+        <v>0.36518838334735831</v>
+      </c>
+      <c r="T2">
+        <f>K2/SUM(J2:L2)</f>
+        <v>0.30029420107514343</v>
+      </c>
+      <c r="U2">
+        <f>L2/(SUM(J2:L2))</f>
+        <v>0.33451741557749831</v>
+      </c>
+      <c r="V2">
+        <f>P2/(SUM(P2:R2))</f>
+        <v>0.17353564472751182</v>
+      </c>
+      <c r="W2">
+        <f>Q2/SUM(P2:R2)</f>
+        <v>8.6854253975304829E-2</v>
+      </c>
+      <c r="X2">
+        <f>R2/SUM(P2:R2)</f>
+        <v>0.7396101012971833</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1099,8 +1159,32 @@
       <c r="R3">
         <v>25.040371417855201</v>
       </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S15" si="0">J3/SUM(J3:L3)</f>
+        <v>0.24888104844141379</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T15" si="1">K3/SUM(J3:L3)</f>
+        <v>0.36531249948153155</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U15" si="2">L3/(SUM(J3:L3))</f>
+        <v>0.38580645207705472</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V15" si="3">P3/(SUM(P3:R3))</f>
+        <v>8.8557187466362028E-2</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W15" si="4">Q3/SUM(P3:R3)</f>
+        <v>0.21144292362921727</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X15" si="5">R3/SUM(P3:R3)</f>
+        <v>0.69999988890442066</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1155,8 +1239,32 @@
       <c r="R4">
         <v>25.204379813901198</v>
       </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>0.40246354334530654</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>0.32110732616783039</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="2"/>
+        <v>0.27642913048686318</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="3"/>
+        <v>0.28325809141099412</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="4"/>
+        <v>0.34958926082134811</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="5"/>
+        <v>0.36715264776765777</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1211,8 +1319,32 @@
       <c r="R5">
         <v>39.9691126879937</v>
       </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>0.18036389677559689</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>0.28358649695899663</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="2"/>
+        <v>0.53604960626540643</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="3"/>
+        <v>0.26468211665440433</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="4"/>
+        <v>0.42831397272439647</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="5"/>
+        <v>0.30700391062119942</v>
+      </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1267,8 +1399,32 @@
       <c r="R6">
         <v>59.474214356211</v>
       </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>0.22275429634732269</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>0.41518039036383991</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="2"/>
+        <v>0.36206531328883734</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="3"/>
+        <v>0.10742957617766262</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="4"/>
+        <v>0.40846714411759882</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="5"/>
+        <v>0.48410327970473849</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1323,8 +1479,32 @@
       <c r="R7">
         <v>40.753375839246701</v>
       </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0.28867825327427599</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>0.41009704685297627</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="2"/>
+        <v>0.30122469987274775</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="3"/>
+        <v>6.344145219503082E-2</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="4"/>
+        <v>0.37221441765472141</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="5"/>
+        <v>0.56434413015024776</v>
+      </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1379,8 +1559,32 @@
       <c r="R8">
         <v>19.027660985094698</v>
       </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>0.50119484105269085</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>0.27811628077239953</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="2"/>
+        <v>0.22068887817490954</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="3"/>
+        <v>0.30402355322384478</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="4"/>
+        <v>5.5845369594462485E-2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="5"/>
+        <v>0.64013107718169271</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1435,8 +1639,32 @@
       <c r="R9">
         <v>47.018018641897299</v>
       </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>0.25603084886223743</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>0.3840937575593632</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="2"/>
+        <v>0.35987539357839932</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="3"/>
+        <v>0.26120577406808082</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="4"/>
+        <v>0.40369025362734895</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="5"/>
+        <v>0.33510397230457029</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1491,8 +1719,32 @@
       <c r="R10">
         <v>8.1774485699522597</v>
       </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>0.47926397164874379</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>0.25765220919381826</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="2"/>
+        <v>0.26308381915743789</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="3"/>
+        <v>0.36953169677809294</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="4"/>
+        <v>0.26753254825636447</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="5"/>
+        <v>0.36293575496554259</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1547,8 +1799,32 @@
       <c r="R11">
         <v>53.5778378443759</v>
       </c>
+      <c r="S11">
+        <f t="shared" si="0"/>
+        <v>0.29939970331958632</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>0.44218370119105188</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="2"/>
+        <v>0.25841659548936174</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="3"/>
+        <v>0.20531759859687645</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="4"/>
+        <v>0.15704338711307833</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="5"/>
+        <v>0.63763901429004521</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1603,8 +1879,32 @@
       <c r="R12">
         <v>23.347038721250701</v>
       </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>0.42826408384443382</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>0.27161489616769352</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>0.30012101998787272</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="3"/>
+        <v>0.16216569380787538</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>0.31073465178066573</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="5"/>
+        <v>0.5270996544114589</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1659,8 +1959,32 @@
       <c r="R13">
         <v>23.208608313642401</v>
       </c>
+      <c r="S13">
+        <f t="shared" si="0"/>
+        <v>0.29946011080716561</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>0.22852881037132469</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>0.47201107882150967</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="3"/>
+        <v>0.12915159499805501</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="4"/>
+        <v>0.23914746241631513</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="5"/>
+        <v>0.63170094258562992</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1715,8 +2039,32 @@
       <c r="R14">
         <v>6.9377145048202298</v>
       </c>
+      <c r="S14">
+        <f t="shared" si="0"/>
+        <v>0.46561640142007715</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>0.27360686162887554</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>0.26077673695104736</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="3"/>
+        <v>0.11468279114173492</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="4"/>
+        <v>0.40166549015199637</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="5"/>
+        <v>0.48365171870626877</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1770,6 +2118,30 @@
       </c>
       <c r="R15">
         <v>59.844001200788099</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="0"/>
+        <v>0.21133276313905749</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>0.31364316997947572</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>0.47502406688146676</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="3"/>
+        <v>0.19450369367338693</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="4"/>
+        <v>0.34775143818558735</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="5"/>
+        <v>0.45774486814102577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>